<commit_message>
Start evaluation and cleaning of documents
</commit_message>
<xml_diff>
--- a/HLS_man/COP19/COP19_man_timor_leste.xlsx
+++ b/HLS_man/COP19/COP19_man_timor_leste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\OneDrive - Delft University of Technology\Documenten\GitHub\TextToDistributiveJustice\HLS_man\COP19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45852625-EDD9-4828-8EBD-464CB8C83086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AA30D1-CA57-4EAD-8691-2272F0904A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>It is a great honour to be here representing the Government o f Timor-Leste at this igi
 session of the Conference of the Parties to the UNFCCC and 9" Meeting of Parties to
@@ -700,8 +700,8 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,6 +1053,9 @@
       <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="F27" t="s">
         <v>50</v>
       </c>

</xml_diff>